<commit_message>
Finished Add Client Screen
</commit_message>
<xml_diff>
--- a/SoftwareAnalysisFinal/data-samples.xlsx
+++ b/SoftwareAnalysisFinal/data-samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mysait-my.sharepoint.com/personal/harry_jung_edu_sait_ca/Documents/Soft Analysis/SoftwareAnalysisFinal/SoftwareAnalysisFinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAC8F31-D8AE-4F2E-939C-3DD2C0F468B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7CAC8F31-D8AE-4F2E-939C-3DD2C0F468B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C30311BD-68A5-4F8F-8377-1AA9B8D9DCA3}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{7C368670-64C0-434E-9DC9-C2214BFBBAEF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>category_id</t>
   </si>
@@ -153,12 +153,6 @@
   </si>
   <si>
     <t>jd@sample.net</t>
-  </si>
-  <si>
-    <t>js@live.com</t>
-  </si>
-  <si>
-    <t>ml@sample.net</t>
   </si>
   <si>
     <t>Rental Information</t>
@@ -573,7 +567,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -802,7 +796,7 @@
         <v>32</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
@@ -819,20 +813,20 @@
         <v>35</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
         <v>24</v>
@@ -841,13 +835,13 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F29" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" t="s">
         <v>44</v>
-      </c>
-      <c r="G29" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
@@ -899,8 +893,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E23" r:id="rId1" xr:uid="{86E15A3B-14AF-4BE1-9D5D-7DAD5089D164}"/>
-    <hyperlink ref="E24" r:id="rId2" xr:uid="{1D941766-B35B-4996-88ED-3DEC7CF42ADC}"/>
-    <hyperlink ref="E25" r:id="rId3" xr:uid="{77C9B948-1599-41AE-ABEF-D6CBDBBF9129}"/>
+    <hyperlink ref="E24:E25" r:id="rId2" display="jd@sample.net" xr:uid="{C29C2A07-3801-42A3-9C11-CDD1F0C77361}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>